<commit_message>
report generator tests and power improved
</commit_message>
<xml_diff>
--- a/server/tests/services/report_generator/reports/power_example.xlsx
+++ b/server/tests/services/report_generator/reports/power_example.xlsx
@@ -469,31 +469,11 @@
           <t>name2</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>name3</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>name4</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>name5</t>
-        </is>
-      </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>name6</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>01/01/2024 10:00:00</t>
+          <t>01/01/2023 10:00:00</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -502,23 +482,11 @@
       <c r="C3" t="n">
         <v>100</v>
       </c>
-      <c r="D3" t="n">
-        <v>100</v>
-      </c>
-      <c r="E3" t="n">
-        <v>100</v>
-      </c>
-      <c r="F3" t="n">
-        <v>100</v>
-      </c>
-      <c r="G3" t="n">
-        <v>100</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>01/01/2024 10:01:00</t>
+          <t>01/01/2023 10:01:00</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -527,41 +495,17 @@
       <c r="C4" t="n">
         <v>101</v>
       </c>
-      <c r="D4" t="n">
-        <v>101</v>
-      </c>
-      <c r="E4" t="n">
-        <v>101</v>
-      </c>
-      <c r="F4" t="n">
-        <v>101</v>
-      </c>
-      <c r="G4" t="n">
-        <v>101</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>01/01/2024 10:02:00</t>
+          <t>01/01/2023 10:02:00</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>102</v>
       </c>
       <c r="C5" t="n">
-        <v>102</v>
-      </c>
-      <c r="D5" t="n">
-        <v>102</v>
-      </c>
-      <c r="E5" t="n">
-        <v>102</v>
-      </c>
-      <c r="F5" t="n">
-        <v>102</v>
-      </c>
-      <c r="G5" t="n">
         <v>102</v>
       </c>
     </row>

</xml_diff>